<commit_message>
added fuel, adjusted import
</commit_message>
<xml_diff>
--- a/example/kerber_landnetz_fl2/scenarios/basic.xlsx
+++ b/example/kerber_landnetz_fl2/scenarios/basic.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/example/kerber_landnetz_fl2/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C37D153-6384-7A44-AB07-1F522BAA21FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08533E8B-BF48-A040-B2F9-1B9C566A5D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="640" windowWidth="28040" windowHeight="17420" activeTab="8" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
+    <workbookView xWindow="1620" yWindow="640" windowWidth="28040" windowHeight="17420" activeTab="7" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="16" r:id="rId1"/>
     <sheet name="load" sheetId="2" r:id="rId2"/>
     <sheet name="asymmetric_load" sheetId="5" r:id="rId3"/>
     <sheet name="motor" sheetId="4" r:id="rId4"/>
-    <sheet name="gen" sheetId="8" r:id="rId5"/>
-    <sheet name="sgen" sheetId="3" r:id="rId6"/>
+    <sheet name="sgen" sheetId="3" r:id="rId5"/>
+    <sheet name="gen" sheetId="8" r:id="rId6"/>
     <sheet name="asymmetric_sgen" sheetId="6" r:id="rId7"/>
-    <sheet name="ext_grid" sheetId="9" r:id="rId8"/>
-    <sheet name="storage" sheetId="7" r:id="rId9"/>
-    <sheet name="trafo" sheetId="10" r:id="rId10"/>
-    <sheet name="trafo3w" sheetId="11" r:id="rId11"/>
-    <sheet name="ward" sheetId="12" r:id="rId12"/>
-    <sheet name="xward" sheetId="13" r:id="rId13"/>
-    <sheet name="trafo_std_types" sheetId="14" r:id="rId14"/>
-    <sheet name="trafo3w_std_types" sheetId="15" r:id="rId15"/>
+    <sheet name="fuel" sheetId="17" r:id="rId8"/>
+    <sheet name="ext_grid" sheetId="9" r:id="rId9"/>
+    <sheet name="storage" sheetId="7" r:id="rId10"/>
+    <sheet name="trafo" sheetId="10" r:id="rId11"/>
+    <sheet name="trafo3w" sheetId="11" r:id="rId12"/>
+    <sheet name="ward" sheetId="12" r:id="rId13"/>
+    <sheet name="xward" sheetId="13" r:id="rId14"/>
+    <sheet name="trafo_std_types" sheetId="14" r:id="rId15"/>
+    <sheet name="trafo3w_std_types" sheetId="15" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="116">
   <si>
     <t>wye</t>
   </si>
@@ -389,6 +390,15 @@
   </si>
   <si>
     <t>household8</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>gen_type</t>
   </si>
 </sst>
 </file>
@@ -806,6 +816,83 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699321C4-99D5-544B-8F83-A7A6C219F50E}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF49ED3A-8BCC-F043-98DC-39A8D142EE40}">
   <dimension ref="A1:X2"/>
   <sheetViews>
@@ -945,7 +1032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03698C73-FE5E-9349-9185-822495C75A6F}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
@@ -1058,7 +1145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B937B77-D550-5442-9E19-D64BB1FAA85E}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1102,7 +1189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8234EC2-F731-1645-87A1-3289074C0200}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -1158,7 +1245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1DAA20-9FE8-A746-9BA7-813A8662382E}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
@@ -2030,7 +2117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D9EE88-502B-5341-A8AD-D80CC2A5901D}">
   <dimension ref="A1:W3"/>
   <sheetViews>
@@ -2686,6 +2773,77 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9B8466-B32E-3A45-A8E8-7E7227ADE1CD}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F748F6D2-7241-B247-A484-1A76AD864F7F}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -2744,77 +2902,6 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9B8466-B32E-3A45-A8E8-7E7227ADE1CD}">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2884,6 +2971,32 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBD217A-CA61-2642-9465-282EBC6087C9}">
+  <dimension ref="B1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446F108F-AC6A-8448-99B0-5E515C432FDC}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2937,81 +3050,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699321C4-99D5-544B-8F83-A7A6C219F50E}">
-  <dimension ref="A1:L9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added opf analysis, clean code, fixed bugs
</commit_message>
<xml_diff>
--- a/example/kerber_landnetz_fl2/scenarios/basic.xlsx
+++ b/example/kerber_landnetz_fl2/scenarios/basic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/example/kerber_landnetz_fl2/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08533E8B-BF48-A040-B2F9-1B9C566A5D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA245BA-DC97-9043-A0C3-9395D10EB6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="640" windowWidth="28040" windowHeight="17420" activeTab="7" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
+    <workbookView xWindow="1620" yWindow="640" windowWidth="28040" windowHeight="17420" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="16" r:id="rId1"/>
@@ -29,6 +29,8 @@
     <sheet name="xward" sheetId="13" r:id="rId14"/>
     <sheet name="trafo_std_types" sheetId="14" r:id="rId15"/>
     <sheet name="trafo3w_std_types" sheetId="15" r:id="rId16"/>
+    <sheet name="pwl_cost" sheetId="18" r:id="rId17"/>
+    <sheet name="poly_cost" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="127">
   <si>
     <t>wye</t>
   </si>
@@ -399,6 +401,39 @@
   </si>
   <si>
     <t>gen_type</t>
+  </si>
+  <si>
+    <t>power_type</t>
+  </si>
+  <si>
+    <t>element</t>
+  </si>
+  <si>
+    <t>et</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>cp0_eur</t>
+  </si>
+  <si>
+    <t>cp1_eur_per_mw</t>
+  </si>
+  <si>
+    <t>cp2_eur_per_mw2</t>
+  </si>
+  <si>
+    <t>cq0_eur</t>
+  </si>
+  <si>
+    <t>cq1_eur_per_mvar</t>
+  </si>
+  <si>
+    <t>cq2_eur_per_mvar2</t>
+  </si>
+  <si>
+    <t>use_opf</t>
   </si>
 </sst>
 </file>
@@ -490,7 +525,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -778,7 +813,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -786,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800EF47C-ADD7-984D-8831-B2BC1EF8921F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -797,16 +832,22 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2337,6 +2378,88 @@
       <c r="W3" s="1">
         <v>1.2</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDBD4E4-D5C5-C44D-838E-811E4542D9C3}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X33" sqref="X33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CFCB42-C580-2249-8C2C-F4F6BA8F5DB3}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X33" sqref="X33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2974,7 +3097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBD217A-CA61-2642-9465-282EBC6087C9}">
   <dimension ref="B1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added error management and messages in executor
</commit_message>
<xml_diff>
--- a/example/kerber_landnetz_fl2/scenarios/basic.xlsx
+++ b/example/kerber_landnetz_fl2/scenarios/basic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/example/kerber_landnetz_fl2/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA245BA-DC97-9043-A0C3-9395D10EB6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13788FAE-E5DE-894A-A6BA-233B967E9109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="640" windowWidth="28040" windowHeight="17420" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
+    <workbookView xWindow="1620" yWindow="640" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="16" r:id="rId1"/>
@@ -823,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800EF47C-ADD7-984D-8831-B2BC1EF8921F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -2470,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A18980-C5F5-904C-A09F-C403C009A87F}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added use_dc in general
</commit_message>
<xml_diff>
--- a/example/kerber_landnetz_fl2/scenarios/basic.xlsx
+++ b/example/kerber_landnetz_fl2/scenarios/basic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/example/kerber_landnetz_fl2/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13788FAE-E5DE-894A-A6BA-233B967E9109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E9D428-0ED8-3048-AF79-CC6591C63424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="640" windowWidth="28040" windowHeight="17420" activeTab="1" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
+    <workbookView xWindow="1620" yWindow="640" windowWidth="28040" windowHeight="17420" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="16" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="128">
   <si>
     <t>wye</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>use_opf</t>
+  </si>
+  <si>
+    <t>use_dc</t>
   </si>
 </sst>
 </file>
@@ -821,18 +824,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800EF47C-ADD7-984D-8831-B2BC1EF8921F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>104</v>
       </c>
@@ -842,12 +846,18 @@
       <c r="C1" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2470,7 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A18980-C5F5-904C-A09F-C403C009A87F}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>